<commit_message>
task 3. orm query
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">c14112e5-4ae3-43bf-948a-481cf26d80c8</t>
   </si>
   <si>
-    <t xml:space="preserve">Меню</t>
+    <t xml:space="preserve">+Меню</t>
   </si>
   <si>
     <t xml:space="preserve">Основное меню</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">8d8be1c0-af4c-49bb-9567-0c4effeb2902</t>
   </si>
   <si>
-    <t xml:space="preserve">Алкогольное меню</t>
+    <t xml:space="preserve">++Алкогольное меню</t>
   </si>
   <si>
     <t xml:space="preserve">Алкогольные напитки</t>
@@ -325,10 +325,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>

</xml_diff>